<commit_message>
added launching script in jupyter folder
</commit_message>
<xml_diff>
--- a/jupyter_notebooks/file/input/switches_v3/network.xlsx
+++ b/jupyter_notebooks/file/input/switches_v3/network.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FBK106\Documents\Repositories\ResiliencyTool\jupyter_notebooks\file\input\switches_v0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FBK106\Documents\Repositories\ResiliencyTool\jupyter_notebooks\file\input\switches_v3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E39DB9-F106-4D67-A435-9ECBAC22EED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49C37B4B-69D8-4475-BF0A-5EED3C47C13B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32025" yWindow="1800" windowWidth="21600" windowHeight="11385" firstSheet="1" activeTab="3" xr2:uid="{D3DCB828-FBC6-4B5F-B916-8216FBF30931}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{D3DCB828-FBC6-4B5F-B916-8216FBF30931}"/>
   </bookViews>
   <sheets>
     <sheet name="simulation" sheetId="12" r:id="rId1"/>
@@ -3201,8 +3201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3272,11 +3272,9 @@
         <v>220</v>
       </c>
       <c r="D2">
-        <f>D3+0.5</f>
         <v>81.400000000000006</v>
       </c>
       <c r="E2">
-        <f>E3</f>
         <v>9.5</v>
       </c>
       <c r="G2">
@@ -3287,12 +3285,6 @@
       </c>
       <c r="I2" s="2" t="s">
         <v>105</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2">
-        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -3326,11 +3318,9 @@
         <v>110</v>
       </c>
       <c r="D4">
-        <f>D3-P2</f>
         <v>79.900000000000006</v>
       </c>
       <c r="E4">
-        <f>E3</f>
         <v>9.5</v>
       </c>
       <c r="G4">
@@ -3351,11 +3341,9 @@
         <v>110</v>
       </c>
       <c r="D5">
-        <f>D4</f>
         <v>79.900000000000006</v>
       </c>
       <c r="E5">
-        <f>E4+Q2</f>
         <v>10.5</v>
       </c>
       <c r="G5">
@@ -3376,11 +3364,9 @@
         <v>110</v>
       </c>
       <c r="D6">
-        <f>D5</f>
         <v>79.900000000000006</v>
       </c>
       <c r="E6">
-        <f>E5+Q2</f>
         <v>11.5</v>
       </c>
       <c r="G6">
@@ -3401,11 +3387,9 @@
         <v>110</v>
       </c>
       <c r="D7">
-        <f>D6</f>
         <v>79.900000000000006</v>
       </c>
       <c r="E7">
-        <f>E6+Q2</f>
         <v>12.5</v>
       </c>
       <c r="G7">
@@ -3426,11 +3410,9 @@
         <v>110</v>
       </c>
       <c r="D8">
-        <f>D6-P2</f>
         <v>78.900000000000006</v>
       </c>
       <c r="E8">
-        <f>E6</f>
         <v>11.5</v>
       </c>
       <c r="G8">
@@ -3451,11 +3433,9 @@
         <v>110</v>
       </c>
       <c r="D9">
-        <f>D8-P2</f>
         <v>77.900000000000006</v>
       </c>
       <c r="E9">
-        <f>E8</f>
         <v>11.5</v>
       </c>
       <c r="G9">
@@ -3476,11 +3456,9 @@
         <v>110</v>
       </c>
       <c r="D10">
-        <f>D9-P2</f>
         <v>76.900000000000006</v>
       </c>
       <c r="E10">
-        <f>E9</f>
         <v>11.5</v>
       </c>
       <c r="G10">
@@ -3501,11 +3479,9 @@
         <v>110</v>
       </c>
       <c r="D11">
-        <f>D4-P2</f>
         <v>78.900000000000006</v>
       </c>
       <c r="E11">
-        <f>E4</f>
         <v>9.5</v>
       </c>
       <c r="G11">
@@ -3526,11 +3502,9 @@
         <v>110</v>
       </c>
       <c r="D12">
-        <f>D11</f>
         <v>78.900000000000006</v>
       </c>
       <c r="E12">
-        <f>E11-Q2</f>
         <v>8.5</v>
       </c>
       <c r="G12">
@@ -3551,11 +3525,9 @@
         <v>110</v>
       </c>
       <c r="D13">
-        <f>D11-P2</f>
         <v>77.900000000000006</v>
       </c>
       <c r="E13">
-        <f>E11</f>
         <v>9.5</v>
       </c>
       <c r="G13">
@@ -3576,11 +3548,9 @@
         <v>110</v>
       </c>
       <c r="D14">
-        <f>D13-P2</f>
         <v>76.900000000000006</v>
       </c>
       <c r="E14">
-        <f>E13</f>
         <v>9.5</v>
       </c>
       <c r="G14">
@@ -3601,11 +3571,9 @@
         <v>110</v>
       </c>
       <c r="D15">
-        <f>D14</f>
         <v>76.900000000000006</v>
       </c>
       <c r="E15">
-        <f>E14-Q2</f>
         <v>8.5</v>
       </c>
       <c r="G15">
@@ -3626,11 +3594,9 @@
         <v>110</v>
       </c>
       <c r="D16">
-        <f>D14-P2</f>
         <v>75.900000000000006</v>
       </c>
       <c r="E16">
-        <f>E14</f>
         <v>9.5</v>
       </c>
       <c r="G16">
@@ -3651,11 +3617,9 @@
         <v>110</v>
       </c>
       <c r="D17">
-        <f>D16</f>
         <v>75.900000000000006</v>
       </c>
       <c r="E17">
-        <f>E16-Q2</f>
         <v>8.5</v>
       </c>
       <c r="G17">
@@ -3676,11 +3640,9 @@
         <v>110</v>
       </c>
       <c r="D18">
-        <f>D16-P2</f>
         <v>74.900000000000006</v>
       </c>
       <c r="E18">
-        <f>E16</f>
         <v>9.5</v>
       </c>
       <c r="G18">
@@ -3701,11 +3663,9 @@
         <v>110</v>
       </c>
       <c r="D19">
-        <f>D9</f>
         <v>77.900000000000006</v>
       </c>
       <c r="E19">
-        <f>E9+Q2</f>
         <v>12.5</v>
       </c>
       <c r="G19">
@@ -3726,11 +3686,9 @@
         <v>110</v>
       </c>
       <c r="D20">
-        <f>D17-P2</f>
         <v>74.900000000000006</v>
       </c>
       <c r="E20">
-        <f>E17</f>
         <v>8.5</v>
       </c>
       <c r="G20">
@@ -3754,7 +3712,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA2B7A3-5BF0-4668-9FF0-C3329253032F}">
   <dimension ref="A1:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>

</xml_diff>